<commit_message>
Integration and unit tests added
</commit_message>
<xml_diff>
--- a/tests/Meet_the_Family bug codex.xlsx
+++ b/tests/Meet_the_Family bug codex.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t xml:space="preserve">Test Name</t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">comment</t>
   </si>
   <si>
+    <t xml:space="preserve">test_members</t>
+  </si>
+  <si>
     <t xml:space="preserve">MTF_UT_0001</t>
   </si>
   <si>
@@ -137,6 +140,24 @@
   </si>
   <si>
     <t xml:space="preserve">test_get_relationship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTF_IT_0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_set_methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTF_IT_0002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_get_relationship_methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_family_tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTF_UT_0019</t>
   </si>
 </sst>
 </file>
@@ -244,13 +265,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
+      <selection pane="topLeft" activeCell="K27" activeCellId="0" sqref="K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27"/>
@@ -268,147 +289,183 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>4</v>
-      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>11</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="0" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
         <v>38</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Integration and unit tests for family_tree.py added
</commit_message>
<xml_diff>
--- a/tests/Meet_the_Family bug codex.xlsx
+++ b/tests/Meet_the_Family bug codex.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
   <si>
     <t xml:space="preserve">Test Name</t>
   </si>
@@ -158,6 +158,27 @@
   </si>
   <si>
     <t xml:space="preserve">MTF_UT_0019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTF_UT_0020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTF_UT_0021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_add_spouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTF_UT_0022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFT_IT_0003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFT_IT_0004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFT_IT_0005</t>
   </si>
 </sst>
 </file>
@@ -265,10 +286,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K27" activeCellId="0" sqref="K27"/>
+      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -468,6 +489,54 @@
         <v>5</v>
       </c>
     </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Finish project, add tests and system test. Added initialization
</commit_message>
<xml_diff>
--- a/tests/Meet_the_Family bug codex.xlsx
+++ b/tests/Meet_the_Family bug codex.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="73">
   <si>
     <t xml:space="preserve">Test Name</t>
   </si>
@@ -142,6 +142,18 @@
     <t xml:space="preserve">test_get_relationship</t>
   </si>
   <si>
+    <t xml:space="preserve">MFT_UT_0023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_get_sinblings_spouses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFT_UT_0024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_get_spouse_siblings</t>
+  </si>
+  <si>
     <t xml:space="preserve">MTF_IT_0001</t>
   </si>
   <si>
@@ -179,6 +191,54 @@
   </si>
   <si>
     <t xml:space="preserve">MFT_IT_0005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_geektrust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTF_UT_0025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_construct_add_child_method_call</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTF_UT_0026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_construct_add_spouse_method_call</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTF_UT_0027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_construct_get_relationship_method_call</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTF_UT_0028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_translate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTF_UT_0029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_execute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTF_UT_0030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTF_UT_0031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test_setup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFT_IT_0006</t>
   </si>
 </sst>
 </file>
@@ -286,13 +346,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27"/>
@@ -477,64 +537,149 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="0" t="s">
         <v>44</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>13</v>
+      <c r="A25" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="0" t="s">
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="0" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>